<commit_message>
Uitproberen Effectivelengths met eccentrische sup
</commit_message>
<xml_diff>
--- a/Examples/GetRFEMData/ExcelGlobalParamTest.xlsx
+++ b/Examples/GetRFEMData/ExcelGlobalParamTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\RFEM_Python_Client_4\Examples\GetRFEMData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reken\PYTHON\RFEM_Python_Client\Examples\GetRFEMData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC84E9CD-5962-493E-B0FE-BF4C5096998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13F3F81E-E813-453D-9F49-5FCB7DC3CBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="3360" windowWidth="16965" windowHeight="11505" activeTab="1" xr2:uid="{4BEEA08F-267C-40A9-9957-7064C9DC3562}"/>
+    <workbookView xWindow="5205" yWindow="2265" windowWidth="21600" windowHeight="12195" activeTab="1" xr2:uid="{4BEEA08F-267C-40A9-9957-7064C9DC3562}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>

</xml_diff>